<commit_message>
Made the Observing FE Results on the Experimental SVM Hyperplanes script
</commit_message>
<xml_diff>
--- a/Depth Damaged States Attenuation Model - Orientation =  90, Width = 2, Circumference = Outside, Axial Location = 235/PCs at A'.xlsx
+++ b/Depth Damaged States Attenuation Model - Orientation =  90, Width = 2, Circumference = Outside, Axial Location = 235/PCs at A'.xlsx
@@ -396,10 +396,10 @@
         <v>7000</v>
       </c>
       <c r="B2">
-        <v>-0.2857829782529795</v>
+        <v>0.05774824518887228</v>
       </c>
       <c r="C2">
-        <v>0.1251746740930746</v>
+        <v>-0.2060744765059519</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>7333.333333333333</v>
       </c>
       <c r="B3">
-        <v>-0.1713641216280674</v>
+        <v>0.1055372139939831</v>
       </c>
       <c r="C3">
-        <v>0.2691628866934457</v>
+        <v>-0.408083955352122</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +418,10 @@
         <v>7666.666666666667</v>
       </c>
       <c r="B4">
-        <v>-0.2672091298857421</v>
+        <v>0.3798973706054365</v>
       </c>
       <c r="C4">
-        <v>0.08885964872219815</v>
+        <v>-0.3148278294410584</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +429,10 @@
         <v>8000</v>
       </c>
       <c r="B5">
-        <v>-0.2037609987188569</v>
+        <v>0.4235863676534892</v>
       </c>
       <c r="C5">
-        <v>-0.3370909558608488</v>
+        <v>0.150870860007224</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +440,10 @@
         <v>8333.333333333334</v>
       </c>
       <c r="B6">
-        <v>-0.343731815768369</v>
+        <v>0.2775228213405452</v>
       </c>
       <c r="C6">
-        <v>-0.3524625223551583</v>
+        <v>0.1888064069125281</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +451,10 @@
         <v>8666.666666666666</v>
       </c>
       <c r="B7">
-        <v>-0.3402266287114395</v>
+        <v>0.4378796684245714</v>
       </c>
       <c r="C7">
-        <v>-0.353055010291595</v>
+        <v>0.2889597687314303</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +462,10 @@
         <v>9000</v>
       </c>
       <c r="B8">
-        <v>-0.3793864944881054</v>
+        <v>0.3597755484573791</v>
       </c>
       <c r="C8">
-        <v>-0.009856245843924048</v>
+        <v>0.1177697475310628</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +473,10 @@
         <v>9333.333333333334</v>
       </c>
       <c r="B9">
-        <v>-0.4017671282786786</v>
+        <v>0.3000578154893521</v>
       </c>
       <c r="C9">
-        <v>-0.1027945017834699</v>
+        <v>-0.3225071420797199</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +484,10 @@
         <v>9666.666666666666</v>
       </c>
       <c r="B10">
-        <v>-0.3336618454222509</v>
+        <v>0.2669392078947819</v>
       </c>
       <c r="C10">
-        <v>0.02231914608510188</v>
+        <v>0.227954464734328</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -495,10 +495,10 @@
         <v>10000</v>
       </c>
       <c r="B11">
-        <v>-0.2269780937474418</v>
+        <v>0.2117912816228028</v>
       </c>
       <c r="C11">
-        <v>0.4251283202836275</v>
+        <v>0.07386406655290037</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10333.33333333333</v>
       </c>
       <c r="B12">
-        <v>-0.06721544753267006</v>
+        <v>0.03113167679696655</v>
       </c>
       <c r="C12">
-        <v>0.2287364523425529</v>
+        <v>-0.4981864887959363</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +517,10 @@
         <v>10666.66666666667</v>
       </c>
       <c r="B13">
-        <v>-0.187401532994686</v>
+        <v>0.2232812776033924</v>
       </c>
       <c r="C13">
-        <v>0.4674712650727001</v>
+        <v>-0.2998044417371674</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +528,10 @@
         <v>11000</v>
       </c>
       <c r="B14">
-        <v>-0.1383694910781134</v>
+        <v>0.009564627465146133</v>
       </c>
       <c r="C14">
-        <v>0.278486136237694</v>
+        <v>-0.144736744432283</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +539,10 @@
         <v>11333.33333333333</v>
       </c>
       <c r="B15">
-        <v>-0.04032849852316302</v>
+        <v>-0.02085174392840274</v>
       </c>
       <c r="C15">
-        <v>0.006838485553286268</v>
+        <v>0.03087857691674713</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +550,10 @@
         <v>11666.66666666667</v>
       </c>
       <c r="B16">
-        <v>-0.07730361676731469</v>
+        <v>0.02642545352386631</v>
       </c>
       <c r="C16">
-        <v>0.01122341979271957</v>
+        <v>0.06385536862668718</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +561,10 @@
         <v>12000</v>
       </c>
       <c r="B17">
-        <v>0.08690005603000782</v>
+        <v>0.07340691703137811</v>
       </c>
       <c r="C17">
-        <v>-0.03171004826778088</v>
+        <v>-0.1030761880196644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>